<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@99cd66b43a203ee2ef2d541e2dd5a92a72f15cb0 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Generic/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Generic/pedalboard-hw-bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="347">
   <si>
     <t>Row</t>
   </si>
@@ -97,6 +97,24 @@
     <t>2</t>
   </si>
   <si>
+    <t>Unpolarized capacitor</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C31 C32</t>
+  </si>
+  <si>
+    <t>27p</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>C9</t>
   </si>
   <si>
@@ -112,7 +130,7 @@
     <t>50V/10%</t>
   </si>
   <si>
-    <t>3</t>
+    <t>4</t>
   </si>
   <si>
     <t>C7 C8</t>
@@ -127,45 +145,51 @@
     <t>187-CL21B103KBANNNC</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Unpolarized capacitor</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>C1 C2 C3 C4 C5 C11</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>C1 C2 C3 C4 C5 C11 C19 C21 C23 C25 C26 C27 C29 C30 C33</t>
   </si>
   <si>
     <t>100n</t>
   </si>
   <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>https://datasheets.kyocera-avx.com/X7RDielectric.pdf</t>
+  </si>
+  <si>
+    <t>1276-1180-1-ND</t>
+  </si>
+  <si>
+    <t>581-08055C104K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/kyocera-avx/KGM21NR71H104KM/6816312</t>
+  </si>
+  <si>
     <t>6</t>
   </si>
   <si>
-    <t>https://datasheets.kyocera-avx.com/X7RDielectric.pdf</t>
-  </si>
-  <si>
-    <t>1276-1180-1-ND</t>
-  </si>
-  <si>
-    <t>581-08055C104K</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/kyocera-avx/KGM21NR71H104KM/6816312</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>C6 C12 C14 C15 C16 C20</t>
+    <t>C22 C24</t>
+  </si>
+  <si>
+    <t>1u</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>C6 C12 C14 C15 C16 C17 C18 C20</t>
   </si>
   <si>
     <t>22u</t>
   </si>
   <si>
+    <t>8</t>
+  </si>
+  <si>
     <t>https://search.murata.co.jp/Ceramy/image/img/A01X/G101/ENG/GRM21BZ71H475ME15-01.pdf</t>
   </si>
   <si>
@@ -196,7 +220,7 @@
     <t>https://www.digikey.ch/de/products/detail/kemet/A768MS277M1GLAE022/12707654</t>
   </si>
   <si>
-    <t>7</t>
+    <t>9</t>
   </si>
   <si>
     <t>ComputeModule4-CM4</t>
@@ -211,7 +235,7 @@
     <t>DF40C-100DS-0.4V</t>
   </si>
   <si>
-    <t>8</t>
+    <t>10</t>
   </si>
   <si>
     <t>Light emitting diode</t>
@@ -229,10 +253,7 @@
     <t>LED_0805_2012Metric</t>
   </si>
   <si>
-    <t>~</t>
-  </si>
-  <si>
-    <t>9</t>
+    <t>11</t>
   </si>
   <si>
     <t>D5</t>
@@ -241,7 +262,7 @@
     <t>LED Y</t>
   </si>
   <si>
-    <t>10</t>
+    <t>12</t>
   </si>
   <si>
     <t>RGB LED with integrated controller</t>
@@ -262,7 +283,7 @@
     <t>https://www.digikey.ch/de/products/detail/adafruit-industries-llc/1655/5154679</t>
   </si>
   <si>
-    <t>11</t>
+    <t>13</t>
   </si>
   <si>
     <t>100V 0.15A standard switching diode, DO-35</t>
@@ -286,7 +307,34 @@
     <t>https://www.digikey.ch/de/products/detail/micro-commercial-co/SM4007PL-TP/1793250</t>
   </si>
   <si>
-    <t>12</t>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Schottky diode, small symbol</t>
+  </si>
+  <si>
+    <t>D_Schottky_Small</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>SS34HF</t>
+  </si>
+  <si>
+    <t>D_SMA</t>
+  </si>
+  <si>
+    <t>https://www.comchiptech.com/admin/files/product/20190514101641.pdf</t>
+  </si>
+  <si>
+    <t>641-2115-1-ND</t>
+  </si>
+  <si>
+    <t>821-SS34LRVG</t>
+  </si>
+  <si>
+    <t>40V/3A</t>
   </si>
   <si>
     <t>20V 1A Schottky Barrier Rectifier Diode, DO-41</t>
@@ -295,43 +343,16 @@
     <t>1N5817</t>
   </si>
   <si>
-    <t>D13</t>
-  </si>
-  <si>
-    <t>SS34HF</t>
-  </si>
-  <si>
-    <t>D_SMA</t>
-  </si>
-  <si>
-    <t>https://www.comchiptech.com/admin/files/product/20190514101641.pdf</t>
+    <t>D8 D9</t>
+  </si>
+  <si>
+    <t>http://www.vishay.com/docs/88525/1n5817.pdf</t>
   </si>
   <si>
     <t>https://www.digikey.ch/de/products/detail/comchip-technology/SS34-HF/10279693</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>Schottky diode, small symbol</t>
-  </si>
-  <si>
-    <t>D_Schottky_Small</t>
-  </si>
-  <si>
-    <t>D7</t>
-  </si>
-  <si>
-    <t>641-2115-1-ND</t>
-  </si>
-  <si>
-    <t>821-SS34LRVG</t>
-  </si>
-  <si>
-    <t>40V/3A</t>
-  </si>
-  <si>
-    <t>14</t>
+    <t>16</t>
   </si>
   <si>
     <t>Resettable fuse, polymeric positive temperature coefficient</t>
@@ -355,7 +376,7 @@
     <t>https://www.digikey.ch/de/products/detail/littelfuse-inc/1812L150-24MR/2023969</t>
   </si>
   <si>
-    <t>15</t>
+    <t>17</t>
   </si>
   <si>
     <t>DC Barrel Jack with an internal switch</t>
@@ -379,7 +400,22 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/694106301002/5047522</t>
   </si>
   <si>
-    <t>16</t>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>Conn_01x02</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>PinHeader_1x02_P2.54mm_Vertical</t>
+  </si>
+  <si>
+    <t>19</t>
   </si>
   <si>
     <t>M Series, 6.35mm (1/4in) stereo jack, switched, with chrome ferrule and straight PCB pins</t>
@@ -403,7 +439,7 @@
     <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
   </si>
   <si>
-    <t>17</t>
+    <t>20</t>
   </si>
   <si>
     <t>Raspberry_Pi_2_3</t>
@@ -424,7 +460,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61304021821/16608657</t>
   </si>
   <si>
-    <t>18</t>
+    <t>21</t>
   </si>
   <si>
     <t>Generic connector, double row, 02x02, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
@@ -442,7 +478,7 @@
     <t>Led-Ring</t>
   </si>
   <si>
-    <t>19</t>
+    <t>22</t>
   </si>
   <si>
     <t>Audio Jack, 3 Poles (Stereo / TRS), Switched TR Poles (Normalling)</t>
@@ -466,7 +502,7 @@
     <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
   </si>
   <si>
-    <t>20</t>
+    <t>23</t>
   </si>
   <si>
     <t>5-pin DIN connector (5-pin DIN-5 stereo)</t>
@@ -490,31 +526,7 @@
     <t>https://www.digikey.ch/de/products/detail/switchcraft-inc/57PC5F/275385</t>
   </si>
   <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>Generic connector, single row, 01x02, script generated</t>
-  </si>
-  <si>
-    <t>Conn_01x02_Pin</t>
-  </si>
-  <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>Pico USB TP</t>
-  </si>
-  <si>
-    <t>Spring_Loaded_Pins_2mm</t>
-  </si>
-  <si>
-    <t>https://media.digikey.com/pdf/Data%20Sheets/Mill%20Max%20PDFs/Spring%20Loaded%20Connectors.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/mill-max-manufacturing-corp/0906-0-15-20-76-14-11-0/1147048</t>
-  </si>
-  <si>
-    <t>22</t>
+    <t>24</t>
   </si>
   <si>
     <t>Generic connector, single row, 01x03, script generated</t>
@@ -538,7 +550,22 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61300311021/4846824</t>
   </si>
   <si>
-    <t>23</t>
+    <t>25</t>
+  </si>
+  <si>
+    <t>USB_B_Micro-Connector</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>USB_B_Micro</t>
+  </si>
+  <si>
+    <t>USB_Micro-B_Amphenol_10104110_Horizontal</t>
+  </si>
+  <si>
+    <t>26</t>
   </si>
   <si>
     <t>Inductor</t>
@@ -562,7 +589,7 @@
     <t>815-ASPI-6045S-120MT</t>
   </si>
   <si>
-    <t>24</t>
+    <t>27</t>
   </si>
   <si>
     <t>Inductor with ferrite core</t>
@@ -586,7 +613,7 @@
     <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
   </si>
   <si>
-    <t>25</t>
+    <t>28</t>
   </si>
   <si>
     <t>FDS4435BZ</t>
@@ -604,7 +631,7 @@
     <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
   </si>
   <si>
-    <t>26</t>
+    <t>29</t>
   </si>
   <si>
     <t>Resistor</t>
@@ -625,7 +652,13 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
   </si>
   <si>
-    <t>27</t>
+    <t>30</t>
+  </si>
+  <si>
+    <t>R10 R11</t>
+  </si>
+  <si>
+    <t>31</t>
   </si>
   <si>
     <t>R3</t>
@@ -640,7 +673,7 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
   </si>
   <si>
-    <t>28</t>
+    <t>32</t>
   </si>
   <si>
     <t>R1 R5</t>
@@ -652,16 +685,13 @@
     <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238 https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT470R/1760300</t>
   </si>
   <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>R2 R6</t>
+    <t>R2 R6 R12 R13 R14 R15</t>
   </si>
   <si>
     <t>1k</t>
   </si>
   <si>
-    <t>30</t>
+    <t>34</t>
   </si>
   <si>
     <t>Resistor, small symbol</t>
@@ -688,7 +718,7 @@
     <t>125mW/1%</t>
   </si>
   <si>
-    <t>31</t>
+    <t>35</t>
   </si>
   <si>
     <t>R8</t>
@@ -703,7 +733,7 @@
     <t>71-CRCW080510K0FKEAC</t>
   </si>
   <si>
-    <t>32</t>
+    <t>36</t>
   </si>
   <si>
     <t>R7</t>
@@ -718,6 +748,9 @@
     <t>71-CRCW0805-12.1K-E3</t>
   </si>
   <si>
+    <t>37</t>
+  </si>
+  <si>
     <t>Omron B3FS 6x6mm single pole normally-open tactile switch</t>
   </si>
   <si>
@@ -739,7 +772,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
   </si>
   <si>
-    <t>34</t>
+    <t>38</t>
   </si>
   <si>
     <t>SW5</t>
@@ -748,13 +781,13 @@
     <t>B</t>
   </si>
   <si>
-    <t>35</t>
+    <t>39</t>
   </si>
   <si>
     <t>SW6</t>
   </si>
   <si>
-    <t>36</t>
+    <t>40</t>
   </si>
   <si>
     <t>SW1</t>
@@ -763,7 +796,7 @@
     <t>D</t>
   </si>
   <si>
-    <t>37</t>
+    <t>41</t>
   </si>
   <si>
     <t>SW2</t>
@@ -772,7 +805,7 @@
     <t>E</t>
   </si>
   <si>
-    <t>38</t>
+    <t>42</t>
   </si>
   <si>
     <t>SW3</t>
@@ -781,7 +814,7 @@
     <t>F</t>
   </si>
   <si>
-    <t>39</t>
+    <t>43</t>
   </si>
   <si>
     <t>Rotary encoder, dual channel, incremental quadrate outputs, with switch</t>
@@ -805,7 +838,7 @@
     <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
   </si>
   <si>
-    <t>40</t>
+    <t>44</t>
   </si>
   <si>
     <t>SW7</t>
@@ -814,7 +847,7 @@
     <t>VOL Rotary</t>
   </si>
   <si>
-    <t>41</t>
+    <t>45</t>
   </si>
   <si>
     <t>74AHCT1G32SE-7</t>
@@ -832,70 +865,118 @@
     <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
   </si>
   <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>Pico</t>
+    <t>46</t>
+  </si>
+  <si>
+    <t>1A Low drop-out regulator, Fixed Output 3.3V, SOT-223</t>
+  </si>
+  <si>
+    <t>NCP1117-3.3_SOT223</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>SOT-223-3_TabPin2</t>
+  </si>
+  <si>
+    <t>http://www.onsemi.com/pub_link/Collateral/NCP1117-D.PDF</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>RP2040</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>RP2040-QFN-56</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
+  </si>
+  <si>
+    <t>TLP2761</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>SO-6L_10x3.84mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3.5V to 28V Input, 3A, Step-Down Converter with Eco-mode(tm)</t>
+  </si>
+  <si>
+    <t>TPS54331</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/tps54331.pdf</t>
+  </si>
+  <si>
+    <t>296-26991-1-ND</t>
+  </si>
+  <si>
+    <t>595-TPS54331DR</t>
+  </si>
+  <si>
+    <t>Can use the tube version 296-23626-5-ND</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>W25Q128JVS-Memory_Flash</t>
   </si>
   <si>
     <t>U1</t>
   </si>
   <si>
-    <t>RPi_Pico_SMD_TH</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/6130xx11121.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/61302011121/4846860</t>
-  </si>
-  <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>15-Mbps inverting photocouple,5 kVrms, 2.7 - 5.5 Vdd, push-pull output</t>
-  </si>
-  <si>
-    <t>TLP2761</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>SO-6L_10x3.84mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3.5V to 28V Input, 3A, Step-Down Converter with Eco-mode(tm)</t>
-  </si>
-  <si>
-    <t>TPS54331</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://www.ti.com/lit/ds/symlink/tps54331.pdf</t>
-  </si>
-  <si>
-    <t>296-26991-1-ND</t>
-  </si>
-  <si>
-    <t>595-TPS54331DR</t>
-  </si>
-  <si>
-    <t>Can use the tube version 296-23626-5-ND</t>
+    <t>W25Q128JVS</t>
+  </si>
+  <si>
+    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>http://www.winbond.com/resource-files/w25q128jv_dtr%20revc%2003272018%20plus.pdf</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>Two pin crystal</t>
+  </si>
+  <si>
+    <t>Crystal</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>ABLS-12.000MHZ-B4-T</t>
+  </si>
+  <si>
+    <t>Crystal_SMD_HC49-US</t>
   </si>
   <si>
     <t>KiBot Bill of Materials</t>
@@ -928,7 +1009,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>7.0.7-7.0.7~ubuntu23.04.1</t>
+    <t>7.0.8-7.0.8~ubuntu23.04.1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -937,13 +1018,13 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>79 (53 SMD/ 24 THT)</t>
+    <t>107 (81 SMD/ 24 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>78 (53 SMD/ 23 THT)</t>
+    <t>104 (80 SMD/ 22 THT)</t>
   </si>
   <si>
     <t>Number of PCBs:</t>
@@ -952,7 +1033,7 @@
     <t>Total Components:</t>
   </si>
   <si>
-    <t>J6</t>
+    <t>J6 J14</t>
   </si>
   <si>
     <t>Debug</t>
@@ -962,6 +1043,12 @@
   </si>
   <si>
     <t xml:space="preserve"> (DNF)</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>DNF</t>
   </si>
   <si>
     <t>KiCad Fields (default)</t>
@@ -1522,7 +1609,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1533,8 +1620,8 @@
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="60.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="59.7109375" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" customWidth="1"/>
     <col min="6" max="6" width="60.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
@@ -1548,7 +1635,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>292</v>
+        <v>319</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1563,55 +1650,55 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>293</v>
+        <v>320</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>294</v>
+        <v>321</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>303</v>
+        <v>330</v>
       </c>
       <c r="F2" s="3">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>295</v>
+        <v>322</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>296</v>
+        <v>323</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>304</v>
+        <v>331</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>305</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>297</v>
+        <v>324</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>298</v>
+        <v>325</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>306</v>
+        <v>333</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>307</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>299</v>
+        <v>326</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>300</v>
+        <v>327</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>308</v>
+        <v>335</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1619,16 +1706,16 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>301</v>
+        <v>328</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>302</v>
+        <v>329</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>309</v>
+        <v>336</v>
       </c>
       <c r="F6" s="3">
-        <v>78</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1718,37 +1805,37 @@
         <v>24</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>18</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" s="10" t="s">
         <v>29</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="M10" s="12" t="s">
         <v>20</v>
@@ -1774,7 +1861,7 @@
         <v>18</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>19</v>
@@ -1789,194 +1876,194 @@
         <v>34</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="M11" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="30" customHeight="1">
+    <row r="12" spans="1:13">
       <c r="A12" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="E12" s="11" t="s">
         <v>38</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>39</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>18</v>
       </c>
       <c r="G12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="K12" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="L12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="M12" s="10" t="s">
-        <v>44</v>
+        <v>35</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="30" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="J13" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="6" t="s">
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="M13" s="6" t="s">
+      <c r="B14" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="30" customHeight="1">
-      <c r="A14" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="10" t="s">
+      <c r="E14" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="F14" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="30" customHeight="1">
+      <c r="A15" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="B15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E15" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="11" t="s">
+      <c r="H15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M14" s="10" t="s">
+      <c r="J15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="6" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="5" t="s">
+      <c r="M15" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="7" t="s">
+    </row>
+    <row r="16" spans="1:13" ht="30" customHeight="1">
+      <c r="A16" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="C16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="7" t="s">
+      <c r="D16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="7" t="s">
+      <c r="E16" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="J15" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="9" t="s">
+      <c r="F16" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>68</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>13</v>
@@ -1984,8 +2071,8 @@
       <c r="H16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="12" t="s">
-        <v>69</v>
+      <c r="I16" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="J16" s="12" t="s">
         <v>20</v>
@@ -1996,28 +2083,28 @@
       <c r="L16" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="M16" s="12" t="s">
-        <v>20</v>
+      <c r="M16" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>64</v>
+        <v>66</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>13</v>
@@ -2025,8 +2112,8 @@
       <c r="H17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="8" t="s">
-        <v>69</v>
+      <c r="I17" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>20</v>
@@ -2041,65 +2128,65 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="30" customHeight="1">
+    <row r="18" spans="1:13">
       <c r="A18" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="D18" s="11" t="s">
         <v>74</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>76</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>75</v>
       </c>
       <c r="F18" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" s="11" t="s">
+      <c r="B19" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="J18" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L18" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M18" s="10" t="s">
+      <c r="E19" s="7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="30" customHeight="1">
-      <c r="A19" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="F19" s="7" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>13</v>
@@ -2107,8 +2194,8 @@
       <c r="H19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="7" t="s">
-        <v>86</v>
+      <c r="I19" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>20</v>
@@ -2119,37 +2206,37 @@
       <c r="L19" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M19" s="6" t="s">
-        <v>87</v>
+      <c r="M19" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="30" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="H20" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="J20" s="12" t="s">
         <v>20</v>
@@ -2161,27 +2248,27 @@
         <v>20</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E21" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>93</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>13</v>
@@ -2190,39 +2277,39 @@
         <v>19</v>
       </c>
       <c r="I21" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M21" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="J21" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="M21" s="8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="30" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>13</v>
@@ -2231,48 +2318,48 @@
         <v>19</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="J22" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K22" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L22" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M22" s="10" t="s">
-        <v>110</v>
+        <v>101</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="L22" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="M22" s="12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="J23" s="8" t="s">
         <v>20</v>
@@ -2284,36 +2371,36 @@
         <v>20</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="J24" s="12" t="s">
         <v>20</v>
@@ -2325,27 +2412,27 @@
         <v>20</v>
       </c>
       <c r="M24" s="10" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>20</v>
+        <v>118</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>13</v>
@@ -2354,7 +2441,7 @@
         <v>19</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="J25" s="8" t="s">
         <v>20</v>
@@ -2366,36 +2453,36 @@
         <v>20</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="45" customHeight="1">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="30" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>19</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="J26" s="12" t="s">
         <v>20</v>
@@ -2412,31 +2499,31 @@
     </row>
     <row r="27" spans="1:13" ht="30" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="J27" s="8" t="s">
         <v>20</v>
@@ -2448,77 +2535,77 @@
         <v>20</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="30" customHeight="1">
       <c r="A28" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L28" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M28" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="45" customHeight="1">
+      <c r="A29" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="D29" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="E29" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="F29" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="E28" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I28" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K28" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L28" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M28" s="10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="30" customHeight="1">
-      <c r="A29" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>161</v>
-      </c>
       <c r="G29" s="5" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I29" s="7" t="s">
-        <v>162</v>
+      <c r="I29" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="J29" s="8" t="s">
         <v>20</v>
@@ -2529,151 +2616,151 @@
       <c r="L29" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M29" s="6" t="s">
-        <v>163</v>
+      <c r="M29" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K30" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L30" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M30" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="30" customHeight="1">
+      <c r="A31" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="F31" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="G31" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I31" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="J31" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L31" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M31" s="6" t="s">
         <v>167</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I30" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="J30" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K30" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L30" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M30" s="10" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="L31" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M31" s="8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K32" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L32" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M32" s="10" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>180</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I32" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="J32" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K32" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L32" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M32" s="10" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="30" customHeight="1">
-      <c r="A33" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>191</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>13</v>
@@ -2681,8 +2768,8 @@
       <c r="H33" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I33" s="7" t="s">
-        <v>192</v>
+      <c r="I33" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="J33" s="8" t="s">
         <v>20</v>
@@ -2693,28 +2780,28 @@
       <c r="L33" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="M33" s="6" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="30" customHeight="1">
+      <c r="M33" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="9" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>73</v>
+        <v>185</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>13</v>
@@ -2722,204 +2809,204 @@
       <c r="H34" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I34" s="11" t="s">
-        <v>199</v>
-      </c>
-      <c r="J34" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K34" s="12" t="s">
-        <v>20</v>
+      <c r="I34" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="K34" s="10" t="s">
+        <v>188</v>
       </c>
       <c r="L34" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="M34" s="10" t="s">
-        <v>200</v>
+      <c r="M34" s="12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L35" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M35" s="6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="30" customHeight="1">
+      <c r="A36" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I36" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="D35" s="7" t="s">
+      <c r="J36" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K36" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L36" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M36" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="E35" s="7" t="s">
+    </row>
+    <row r="37" spans="1:13" ht="30" customHeight="1">
+      <c r="A37" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="F35" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G35" s="5" t="s">
+      <c r="B37" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G37" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H35" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="J35" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K35" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L35" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M35" s="6" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="60" customHeight="1">
-      <c r="A36" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="E36" s="11" t="s">
+      <c r="H37" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I37" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="F36" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I36" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="J36" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K36" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L36" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M36" s="10" t="s">
+      <c r="J37" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K37" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L37" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M37" s="6" t="s">
         <v>209</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K37" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L37" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M37" s="8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K38" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L38" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M38" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="30" customHeight="1">
+      <c r="A39" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D39" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="E39" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="C38" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I38" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="J38" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="K38" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="L38" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="M38" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>224</v>
-      </c>
       <c r="F39" s="7" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>13</v>
@@ -2927,122 +3014,122 @@
       <c r="H39" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I39" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J39" s="6" t="s">
+      <c r="I39" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K39" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L39" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="60" customHeight="1">
+      <c r="A40" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="J40" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K40" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L40" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M40" s="10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K41" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L41" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M41" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C42" s="11" t="s">
         <v>225</v>
       </c>
-      <c r="K39" s="6" t="s">
+      <c r="D42" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="L39" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="M39" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="9" t="s">
+      <c r="E42" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="F40" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I40" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="J40" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="K40" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="L40" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="M40" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" ht="30" customHeight="1">
-      <c r="A41" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>235</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I41" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="J41" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K41" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L41" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M41" s="6" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" ht="30" customHeight="1">
-      <c r="A42" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="E42" s="11" t="s">
-        <v>241</v>
-      </c>
       <c r="F42" s="11" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>13</v>
@@ -3051,39 +3138,39 @@
         <v>19</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="J42" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K42" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L42" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M42" s="10" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="30" customHeight="1">
+        <v>228</v>
+      </c>
+      <c r="J42" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="K42" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="L42" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="M42" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" s="5" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="C43" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D43" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>243</v>
-      </c>
       <c r="E43" s="7" t="s">
-        <v>37</v>
+        <v>234</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>13</v>
@@ -3091,40 +3178,40 @@
       <c r="H43" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I43" s="7" t="s">
+      <c r="I43" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="M43" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="J43" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K43" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L43" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M43" s="6" t="s">
+      <c r="B44" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="D44" s="11" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" ht="30" customHeight="1">
-      <c r="A44" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>245</v>
-      </c>
       <c r="E44" s="11" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>13</v>
@@ -3133,39 +3220,39 @@
         <v>19</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="J44" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K44" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="L44" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M44" s="10" t="s">
-        <v>238</v>
+        <v>228</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="K44" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="L44" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="M44" s="12" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="F45" s="7" t="s">
         <v>247</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>236</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>13</v>
@@ -3174,7 +3261,7 @@
         <v>19</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="J45" s="8" t="s">
         <v>20</v>
@@ -3186,7 +3273,7 @@
         <v>20</v>
       </c>
       <c r="M45" s="6" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="30" customHeight="1">
@@ -3194,10 +3281,10 @@
         <v>250</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>251</v>
@@ -3206,7 +3293,7 @@
         <v>252</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>13</v>
@@ -3215,7 +3302,7 @@
         <v>19</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="J46" s="12" t="s">
         <v>20</v>
@@ -3227,7 +3314,7 @@
         <v>20</v>
       </c>
       <c r="M46" s="10" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="30" customHeight="1">
@@ -3235,19 +3322,19 @@
         <v>253</v>
       </c>
       <c r="B47" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="D47" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="C47" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>256</v>
-      </c>
       <c r="E47" s="7" t="s">
-        <v>257</v>
+        <v>26</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>13</v>
@@ -3256,7 +3343,7 @@
         <v>19</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="J47" s="8" t="s">
         <v>20</v>
@@ -3268,27 +3355,27 @@
         <v>20</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="30" customHeight="1">
       <c r="A48" s="9" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>13</v>
@@ -3297,7 +3384,7 @@
         <v>19</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="J48" s="12" t="s">
         <v>20</v>
@@ -3309,36 +3396,36 @@
         <v>20</v>
       </c>
       <c r="M48" s="10" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>20</v>
+        <v>258</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>243</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>19</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="J49" s="8" t="s">
         <v>20</v>
@@ -3350,27 +3437,27 @@
         <v>20</v>
       </c>
       <c r="M49" s="6" t="s">
-        <v>269</v>
+        <v>249</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="30" customHeight="1">
       <c r="A50" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>20</v>
+        <v>261</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>243</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>271</v>
+        <v>244</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>273</v>
+        <v>247</v>
       </c>
       <c r="G50" s="9" t="s">
         <v>13</v>
@@ -3379,7 +3466,7 @@
         <v>19</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>274</v>
+        <v>248</v>
       </c>
       <c r="J50" s="12" t="s">
         <v>20</v>
@@ -3391,27 +3478,27 @@
         <v>20</v>
       </c>
       <c r="M50" s="10" t="s">
-        <v>275</v>
+        <v>249</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="30" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>13</v>
@@ -3420,7 +3507,7 @@
         <v>19</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="J51" s="8" t="s">
         <v>20</v>
@@ -3432,27 +3519,27 @@
         <v>20</v>
       </c>
       <c r="M51" s="6" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="30" customHeight="1">
       <c r="A52" s="9" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>284</v>
+        <v>265</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>285</v>
+        <v>266</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>287</v>
+        <v>269</v>
       </c>
       <c r="G52" s="9" t="s">
         <v>13</v>
@@ -3461,18 +3548,305 @@
         <v>19</v>
       </c>
       <c r="I52" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="J52" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K52" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L52" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M52" s="10" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="30" customHeight="1">
+      <c r="A53" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I53" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="J53" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K53" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L53" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M53" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H54" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I54" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="J54" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K54" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L54" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M54" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C55" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="J52" s="10" t="s">
+      <c r="D55" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="K52" s="10" t="s">
+      <c r="E55" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="F55" s="7" t="s">
         <v>290</v>
       </c>
-      <c r="L52" s="10" t="s">
+      <c r="G55" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I55" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J55" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K55" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L55" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M55" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="30" customHeight="1">
+      <c r="A56" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="M52" s="12" t="s">
+      <c r="B56" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H56" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I56" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="J56" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K56" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L56" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M56" s="10" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="30" customHeight="1">
+      <c r="A57" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="J57" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="K57" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="L57" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="M57" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="30" customHeight="1">
+      <c r="A58" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="B58" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I58" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="J58" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K58" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L58" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M58" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="A59" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I59" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J59" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K59" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L59" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M59" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3488,7 +3862,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -3514,7 +3888,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>292</v>
+        <v>319</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -3529,55 +3903,55 @@
     </row>
     <row r="2" spans="1:13">
       <c r="C2" s="2" t="s">
-        <v>293</v>
+        <v>320</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>294</v>
+        <v>321</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>303</v>
+        <v>330</v>
       </c>
       <c r="F2" s="3">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="C3" s="2" t="s">
-        <v>295</v>
+        <v>322</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>296</v>
+        <v>323</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>304</v>
+        <v>331</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>305</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="C4" s="2" t="s">
-        <v>297</v>
+        <v>324</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>298</v>
+        <v>325</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>306</v>
+        <v>333</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>307</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="C5" s="2" t="s">
-        <v>299</v>
+        <v>326</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>300</v>
+        <v>327</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>308</v>
+        <v>335</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -3585,16 +3959,16 @@
     </row>
     <row r="6" spans="1:13">
       <c r="C6" s="2" t="s">
-        <v>301</v>
+        <v>328</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>302</v>
+        <v>329</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>309</v>
+        <v>336</v>
       </c>
       <c r="F6" s="3">
-        <v>78</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -3643,39 +4017,80 @@
         <v>13</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>310</v>
+        <v>337</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>311</v>
+        <v>338</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>312</v>
+        <v>339</v>
       </c>
       <c r="G9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>341</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M9" s="8" t="s">
+      <c r="H10" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3702,22 +4117,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="7" t="s">
-        <v>314</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="5" t="s">
-        <v>315</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="6" t="s">
-        <v>316</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>317</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to main from @ pedalboard/pedalboard-hw@3e564fbe2b0c8af9d4b01cda835b757f02c8b2b3 🚀
</commit_message>
<xml_diff>
--- a/latest/BoM/Generic/pedalboard-hw-bom.xlsx
+++ b/latest/BoM/Generic/pedalboard-hw-bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="344">
   <si>
     <t>Row</t>
   </si>
@@ -103,7 +103,7 @@
     <t>C11 C25</t>
   </si>
   <si>
-    <t>27p</t>
+    <t>18p</t>
   </si>
   <si>
     <t>3</t>
@@ -142,789 +142,756 @@
     <t>5</t>
   </si>
   <si>
-    <t>C1 C13 C15 C16 C17 C18 C19 C20 C21 C23 C30 C35</t>
+    <t>C1 C13 C15 C16 C17 C18 C19 C20 C21 C23 C30 C35 C46 C47 C48 C49</t>
   </si>
   <si>
     <t>100n</t>
   </si>
   <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B104KBCNNNC/3886661</t>
+  </si>
+  <si>
+    <t>10% 16V Ceramic Capacitor X7R</t>
+  </si>
+  <si>
+    <t>1276-1180-1-ND</t>
+  </si>
+  <si>
+    <t>581-08055C104K</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>C12 C14</t>
+  </si>
+  <si>
+    <t>1u</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B105KAFNNNE/3886724</t>
+  </si>
+  <si>
+    <t>25V/10%</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>C2 C3 C4 C5 C6 C7 C8 C9 C10 C24 C27 C28 C32 C36 C37 C38 C39 C40 C41 C42 C44 C45</t>
+  </si>
+  <si>
+    <t>10u</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21X106KAYNNNE/5961182</t>
+  </si>
+  <si>
+    <t>10% or 20% 35V Ceramic Capacitor X6S 0805 (2012 Metric)</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>C33 C43</t>
+  </si>
+  <si>
+    <t>100u</t>
+  </si>
+  <si>
+    <t>CP_EIA-7343-31_Kemet-D</t>
+  </si>
+  <si>
+    <t>https://industrial.panasonic.com/cdbs/www-data/pdf/ABE0000/ABE0000C49.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/panasonic-electronic-components/EEF-CX0J101R/816418</t>
+  </si>
+  <si>
+    <t>Capacitor, SP-Cap, 100u, 6.3V, 15mR ESR</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>CM4</t>
+  </si>
+  <si>
+    <t>CM1</t>
+  </si>
+  <si>
+    <t>Raspberry-Pi-4-Compute-Module</t>
+  </si>
+  <si>
+    <t>https://www.hirose.com/en/product/document?clcode=&amp;productname=&amp;series=DF40&amp;documenttype=Catalog&amp;lang=en&amp;documentid=en_DF40_CAT</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/hirose-electric-co-ltd/DF40C-100DS-0-4V-51/1969476</t>
+  </si>
+  <si>
+    <t>DF40C-100DS-0.4V(51)</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>LED R</t>
+  </si>
+  <si>
+    <t>LED_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>D2 D6</t>
+  </si>
+  <si>
+    <t>LED Y</t>
+  </si>
+  <si>
     <t>12</t>
   </si>
   <si>
-    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B104KBCNNNC/3886661</t>
-  </si>
-  <si>
-    <t>10% 16V Ceramic Capacitor X7R</t>
-  </si>
-  <si>
-    <t>1276-1180-1-ND</t>
-  </si>
-  <si>
-    <t>581-08055C104K</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>C12 C14</t>
-  </si>
-  <si>
-    <t>1u</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21B105KAFNNNE/3886724</t>
-  </si>
-  <si>
-    <t>25V/10%</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>C2 C3 C4 C5 C6 C7 C8 C9 C10 C24 C27 C28 C32 C36 C37 C38 C39 C40 C41 C42</t>
-  </si>
-  <si>
-    <t>10u</t>
+    <t>1N4148</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>SM4007</t>
+  </si>
+  <si>
+    <t>D_SOD-123F</t>
+  </si>
+  <si>
+    <t>https://www.mccsemi.com/pdf/Products/SM4001PL-SM4007PL(SOD-123FL).PDF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/micro-commercial-co/SM4007PL-TP/1793250</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Polyfuse</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Polyfuse 1.8A</t>
+  </si>
+  <si>
+    <t>Fuse_1812_4532Metric</t>
+  </si>
+  <si>
+    <t>https://www.littelfuse.com/~/media/electronics/datasheets/resettable_ptcs/littelfuse_ptc_1812l_datasheet.pdf.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/littelfuse-inc/1812L150-24MR/2023969</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Conn_01x03_Pin</t>
+  </si>
+  <si>
+    <t>J28</t>
+  </si>
+  <si>
+    <t>JST PH 3</t>
+  </si>
+  <si>
+    <t>JST_PH_B3B-PH-SM4-TB_1x03-1MP_P2.00mm_Vertical</t>
+  </si>
+  <si>
+    <t>https://www.jst-mfg.com/product/pdf/eng/ePH.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/B3B-PH-K-S/926612</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Conn_01x04_Pin</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>JST PH 4</t>
+  </si>
+  <si>
+    <t>JST_PH_B4B-PH-SM4-TB_1x04-1MP_P2.00mm_Vertical</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/jst-sales-america-inc./B4B-PH-SM4-TB/926833</t>
+  </si>
+  <si>
+    <t>AudioJack3_SwitchTR</t>
+  </si>
+  <si>
+    <t>J1 J3</t>
+  </si>
+  <si>
+    <t>Jack 3.5mm</t>
+  </si>
+  <si>
+    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
+  </si>
+  <si>
+    <t>MIDI Out</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>NMJ6HCD2</t>
+  </si>
+  <si>
+    <t>J5 J8 J18 J19 J20 J22</t>
+  </si>
+  <si>
+    <t>Jack 6.35mm</t>
+  </si>
+  <si>
+    <t>Jack_6.35mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
+  </si>
+  <si>
+    <t>EXP1 EXP2 Audio IN Right Audio OUT Left Audio OUT Right Audio IN Left</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Raspberry_Sound_Card</t>
+  </si>
+  <si>
+    <t>J27</t>
+  </si>
+  <si>
+    <t>Pedalboard Soundcard</t>
+  </si>
+  <si>
+    <t>Pedalboard_Soundcard</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Screw_Terminal_01x02</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>TerminalBlock_Phoenix_MKDS-1,5-2_1x02_P5.00mm_Horizontal</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/phoenix-contact/1715022/260626</t>
   </si>
   <si>
     <t>20</t>
   </si>
   <si>
-    <t>https://www.digikey.ch/de/products/detail/samsung-electro-mechanics/CL21X106KAYNNNE/5961182</t>
-  </si>
-  <si>
-    <t>10% or 20% 35V Ceramic Capacitor X6S 0805 (2012 Metric)</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>CP</t>
-  </si>
-  <si>
-    <t>C33 C43</t>
-  </si>
-  <si>
-    <t>100u</t>
-  </si>
-  <si>
-    <t>CP_EIA-7343-31_Kemet-D</t>
-  </si>
-  <si>
-    <t>https://industrial.panasonic.com/cdbs/www-data/pdf/ABE0000/ABE0000C49.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/panasonic-electronic-components/EEF-CX0J101R/816418</t>
-  </si>
-  <si>
-    <t>Capacitor, SP-Cap, 100u, 6.3V, 15mR ESR</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>CM4</t>
-  </si>
-  <si>
-    <t>CM1</t>
-  </si>
-  <si>
-    <t>Raspberry-Pi-4-Compute-Module</t>
-  </si>
-  <si>
-    <t>https://www.hirose.com/en/product/document?clcode=&amp;productname=&amp;series=DF40&amp;documenttype=Catalog&amp;lang=en&amp;documentid=en_DF40_CAT</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/hirose-electric-co-ltd/DF40C-100DS-0-4V-51/1969476</t>
-  </si>
-  <si>
-    <t>DF40C-100DS-0.4V(51)</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>LED</t>
-  </si>
-  <si>
-    <t>D7</t>
-  </si>
-  <si>
-    <t>LED R</t>
-  </si>
-  <si>
-    <t>LED_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>~</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>D2 D6</t>
-  </si>
-  <si>
-    <t>LED Y</t>
-  </si>
-  <si>
-    <t>1N4148</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>SM4007</t>
-  </si>
-  <si>
-    <t>D_SOD-123F</t>
-  </si>
-  <si>
-    <t>https://www.mccsemi.com/pdf/Products/SM4001PL-SM4007PL(SOD-123FL).PDF</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/micro-commercial-co/SM4007PL-TP/1793250</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>SS34HF</t>
-  </si>
-  <si>
-    <t>D4 D5</t>
-  </si>
-  <si>
-    <t>D_SMA</t>
-  </si>
-  <si>
-    <t>https://www.comchiptech.com/admin/files/product/20190514101641.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/comchip-technology/SS34-HF/10279693</t>
-  </si>
-  <si>
-    <t>40V/3A</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>Polyfuse</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>Polyfuse 1.8A</t>
-  </si>
-  <si>
-    <t>Fuse_1812_4532Metric</t>
-  </si>
-  <si>
-    <t>https://www.littelfuse.com/~/media/electronics/datasheets/resettable_ptcs/littelfuse_ptc_1812l_datasheet.pdf.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/littelfuse-inc/1812L150-24MR/2023969</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>Conn_01x03_Pin</t>
-  </si>
-  <si>
-    <t>J28</t>
-  </si>
-  <si>
-    <t>JST PH 3</t>
-  </si>
-  <si>
-    <t>JST_PH_B3B-PH-SM4-TB_1x03-1MP_P2.00mm_Vertical</t>
-  </si>
-  <si>
-    <t>https://www.jst-mfg.com/product/pdf/eng/ePH.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/jst-sales-america-inc/B3B-PH-K-S/926612</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>Conn_01x04_Pin</t>
-  </si>
-  <si>
-    <t>J14</t>
-  </si>
-  <si>
-    <t>JST PH 4</t>
-  </si>
-  <si>
-    <t>JST_PH_B4B-PH-SM4-TB_1x04-1MP_P2.00mm_Vertical</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/jst-sales-america-inc./B4B-PH-SM4-TB/926833</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
-    <t>AudioJack3_SwitchTR</t>
-  </si>
-  <si>
-    <t>J1 J3</t>
-  </si>
-  <si>
-    <t>Jack 3.5mm</t>
-  </si>
-  <si>
-    <t>Jack_3.5mm_CUI_SJ1-3525N_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.cuidevices.com/product/resource/sj1-352xng.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/cui-devices/SJ1-3525NG/738690</t>
-  </si>
-  <si>
-    <t>MIDI Out</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>NMJ6HCD2</t>
-  </si>
-  <si>
-    <t>J5 J8 J18 J19 J20 J22</t>
-  </si>
-  <si>
-    <t>Jack 6.35mm</t>
-  </si>
-  <si>
-    <t>Jack_6.35mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.schurter.com/en/datasheet/typ_4833.2320.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/schurter-inc/4833-2320/2644235</t>
-  </si>
-  <si>
-    <t>EXP1 EXP2 Audio IN Right Audio OUT Left Audio OUT Right Audio IN Left</t>
-  </si>
-  <si>
-    <t>19</t>
-  </si>
-  <si>
-    <t>Raspberry_Sound_Card</t>
-  </si>
-  <si>
-    <t>J27</t>
-  </si>
-  <si>
-    <t>Pedalboard Soundcard</t>
-  </si>
-  <si>
-    <t>Pedalboard_Soundcard</t>
-  </si>
-  <si>
-    <t>Screw_Terminal_01x02</t>
-  </si>
-  <si>
-    <t>J6</t>
-  </si>
-  <si>
-    <t>TerminalBlock_Phoenix_MKDS-1,5-2_1x02_P5.00mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/phoenix-contact/1715022/260626</t>
+    <t>USB Type A connector</t>
+  </si>
+  <si>
+    <t>USB_A</t>
+  </si>
+  <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>USB_A_Molex_67643_Horizontal</t>
   </si>
   <si>
     <t>21</t>
   </si>
   <si>
-    <t>USB Type A connector, stacked</t>
-  </si>
-  <si>
-    <t>USB_A_Stacked</t>
-  </si>
-  <si>
-    <t>J10</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>USB_B_Micro</t>
-  </si>
-  <si>
-    <t>J11</t>
-  </si>
-  <si>
-    <t>USB_Micro-B_Wuerth_614105150721_Vertical</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/614105150721.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/614105150721/5047749</t>
+    <t>USB mini/micro connector</t>
+  </si>
+  <si>
+    <t>USB_OTG</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>USB_Micro-B_Amphenol_10103594-0001LF_Horizontal</t>
+  </si>
+  <si>
+    <t>L_Ferrite</t>
+  </si>
+  <si>
+    <t>L1 L2 L3 L4</t>
+  </si>
+  <si>
+    <t>120_100MHz</t>
+  </si>
+  <si>
+    <t>L_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
   </si>
   <si>
     <t>23</t>
   </si>
   <si>
-    <t>USB mini/micro connector</t>
-  </si>
-  <si>
-    <t>USB_OTG</t>
-  </si>
-  <si>
-    <t>J9</t>
+    <t>INDUCTOR</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>SRN6045TA-3R3Y</t>
+  </si>
+  <si>
+    <t>L_Bourns_SRN6045TA</t>
+  </si>
+  <si>
+    <t>https://www.bourns.com/docs/Product-Datasheets/SRN6045TA.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/bourns-inc/SRN6045TA-3R3Y/6155103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3µH Semi-Shielded Wirewound Inductor 7.8A 21mOhm Nonstandard </t>
   </si>
   <si>
     <t>24</t>
   </si>
   <si>
-    <t>L_Ferrite</t>
-  </si>
-  <si>
-    <t>L1 L2 L3 L4</t>
-  </si>
-  <si>
-    <t>120_100MHz</t>
-  </si>
-  <si>
-    <t>L_0603_1608Metric</t>
-  </si>
-  <si>
-    <t>https://www.murata.com/products/productdata/8796738650142/ENFA0003.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/murata-electronics/BLM18KG121TN1D/1982762</t>
+    <t>FDS4435BZ</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>SO08-E3</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pdf/datasheet/fds4435bz_f085-d.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
   </si>
   <si>
     <t>25</t>
   </si>
   <si>
-    <t>INDUCTOR</t>
-  </si>
-  <si>
-    <t>L5</t>
-  </si>
-  <si>
-    <t>SRN6045TA-3R3Y</t>
-  </si>
-  <si>
-    <t>L_Bourns_SRN6045TA</t>
-  </si>
-  <si>
-    <t>https://www.bourns.com/docs/Product-Datasheets/SRN6045TA.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/bourns-inc/SRN6045TA-3R3Y/6155103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.3µH Semi-Shielded Wirewound Inductor 7.8A 21mOhm Nonstandard </t>
+    <t>R_Small</t>
+  </si>
+  <si>
+    <t>R5 R13</t>
+  </si>
+  <si>
+    <t>10R</t>
+  </si>
+  <si>
+    <t>R_0805_2012Metric</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
+  </si>
+  <si>
+    <t>Resistor 10R 1% 63mW</t>
   </si>
   <si>
     <t>26</t>
   </si>
   <si>
-    <t>FDS4435BZ</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>SO08-E3</t>
-  </si>
-  <si>
-    <t>https://www.onsemi.com/pdf/datasheet/fds4435bz_f085-d.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/onsemi/FDS4435BZ/1305763</t>
+    <t>R6 R10</t>
+  </si>
+  <si>
+    <t>27R</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
   </si>
   <si>
     <t>27</t>
   </si>
   <si>
-    <t>R_Small</t>
-  </si>
-  <si>
-    <t>R5 R13</t>
-  </si>
-  <si>
-    <t>10R</t>
-  </si>
-  <si>
-    <t>R_0805_2012Metric</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rncp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD10R0/2240197</t>
-  </si>
-  <si>
-    <t>Resistor 10R 1% 63mW</t>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>33R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
   </si>
   <si>
     <t>28</t>
   </si>
   <si>
-    <t>R6 R10</t>
-  </si>
-  <si>
-    <t>27R</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/catalog/sei-rmcf_rmcp.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
+    <t>R3 R7 R20</t>
+  </si>
+  <si>
+    <t>220R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
   </si>
   <si>
     <t>29</t>
   </si>
   <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>33R</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT33R0/1760586</t>
+    <t>R1 R2 R8 R11 R16 R21</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229 https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
   </si>
   <si>
     <t>30</t>
   </si>
   <si>
-    <t>R3 R7 R20</t>
-  </si>
-  <si>
-    <t>220R</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT220R/1760238</t>
+    <t>R15 R17 R22 R23</t>
+  </si>
+  <si>
+    <t>2K2</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT2K20/1760345 https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
+  </si>
+  <si>
+    <t>Resistor 2.2K 1% 63mW</t>
   </si>
   <si>
     <t>31</t>
   </si>
   <si>
-    <t>R1 R2 R8 R11 R16 R21</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229 https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT27R0/1712920</t>
+    <t>R18 R19</t>
+  </si>
+  <si>
+    <t>3K9</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT3K90/1760599</t>
   </si>
   <si>
     <t>32</t>
   </si>
   <si>
-    <t>R15 R17 R22 R23</t>
-  </si>
-  <si>
-    <t>2K2</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT2K20/1760345 https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
-  </si>
-  <si>
-    <t>Resistor 2.2K 1% 63mW</t>
+    <t>R12 R24</t>
+  </si>
+  <si>
+    <t>12K</t>
+  </si>
+  <si>
+    <t>https://www.seielect.com/Catalog/SEI-rmef.PDF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
+  </si>
+  <si>
+    <t>Resistor 12K 1% 63mW</t>
   </si>
   <si>
     <t>33</t>
   </si>
   <si>
-    <t>R18 R19</t>
-  </si>
-  <si>
-    <t>3K9</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT3K90/1760599</t>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>20K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT20K0/1760314</t>
+  </si>
+  <si>
+    <t>Resistor 20K 1% 63mW</t>
   </si>
   <si>
     <t>34</t>
   </si>
   <si>
-    <t>R12 R24</t>
-  </si>
-  <si>
-    <t>12K</t>
-  </si>
-  <si>
-    <t>https://www.seielect.com/Catalog/SEI-rmef.PDF</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RNCP0805FTD1K00/2240229</t>
-  </si>
-  <si>
-    <t>Resistor 12K 1% 63mW</t>
+    <t>R25 R26 R27 R28 R29</t>
+  </si>
+  <si>
+    <t>36K</t>
   </si>
   <si>
     <t>35</t>
   </si>
   <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>20K</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/stackpole-electronics-inc/RMCF0805FT20K0/1760314</t>
-  </si>
-  <si>
-    <t>Resistor 20K 1% 63mW</t>
+    <t>RotaryEncoder_Switch</t>
+  </si>
+  <si>
+    <t>SW1 SW2</t>
+  </si>
+  <si>
+    <t>Rotary</t>
+  </si>
+  <si>
+    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
+  </si>
+  <si>
+    <t>VOL GAIN</t>
   </si>
   <si>
     <t>36</t>
   </si>
   <si>
-    <t>R25 R26 R27 R28 R29</t>
-  </si>
-  <si>
-    <t>36K</t>
+    <t>SW_Omron_B3FS</t>
+  </si>
+  <si>
+    <t>SW5 SW6 SW7 SW8 SW9 SW10</t>
+  </si>
+  <si>
+    <t>Tactile Button</t>
+  </si>
+  <si>
+    <t>SW_PUSH-12mm_Wuerth</t>
+  </si>
+  <si>
+    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
+  </si>
+  <si>
+    <t>D E F A B C</t>
   </si>
   <si>
     <t>37</t>
   </si>
   <si>
-    <t>RotaryEncoder_Switch</t>
-  </si>
-  <si>
-    <t>SW1 SW2</t>
-  </si>
-  <si>
-    <t>Rotary</t>
-  </si>
-  <si>
-    <t>RotaryEncoder_Alps_EC11E-Switch_Vertical_H20mm_CircularMountingHoles</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/482016514001.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/482016514001/10056402</t>
-  </si>
-  <si>
-    <t>VOL GAIN</t>
+    <t>74AHCT1G32SE-7</t>
+  </si>
+  <si>
+    <t>U1 U7</t>
+  </si>
+  <si>
+    <t>SOT-353_SC-70-5</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
   </si>
   <si>
     <t>38</t>
   </si>
   <si>
-    <t>SW_Omron_B3FS</t>
-  </si>
-  <si>
-    <t>SW5 SW6 SW7 SW8 SW9 SW10</t>
-  </si>
-  <si>
-    <t>Tactile Button</t>
-  </si>
-  <si>
-    <t>SW_PUSH-12mm_Wuerth</t>
-  </si>
-  <si>
-    <t>https://www.we-online.com/components/products/datasheet/430172043816.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/w%C3%BCrth-elektronik/430162043826/9950802</t>
-  </si>
-  <si>
-    <t>D E F A B C</t>
+    <t>AP2553W6</t>
+  </si>
+  <si>
+    <t>U10</t>
+  </si>
+  <si>
+    <t>SOT-23-6</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AP255x.pdf</t>
+  </si>
+  <si>
+    <t>AP2553W6-7DICT-ND</t>
   </si>
   <si>
     <t>39</t>
   </si>
   <si>
-    <t>74AHCT1G32SE-7</t>
-  </si>
-  <si>
-    <t>U1 U7</t>
-  </si>
-  <si>
-    <t>SOT-353_SC-70-5</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/74AHCT1G32.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/74AHCT1G32SE-7/2711987</t>
+    <t>AP64351</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>AP64501SP-13</t>
+  </si>
+  <si>
+    <t>SOIC-8-1EP_3.9x4.9mm_P1.27mm_EP2.95x4.9mm_Mask2.71x3.4mm_ThermalVias</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AP64501.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AP64501SP-13/10419715</t>
   </si>
   <si>
     <t>40</t>
   </si>
   <si>
-    <t>AP2553W6</t>
-  </si>
-  <si>
-    <t>U10</t>
-  </si>
-  <si>
-    <t>SOT-23-6</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AP255x.pdf</t>
-  </si>
-  <si>
-    <t>AP2553W6-7DICT-ND</t>
+    <t>Low-Power, Two-Port, High-Speed, USB2.0 (480Mbps) or UART Switch, MSOP-10</t>
+  </si>
+  <si>
+    <t>FSUSB42MUX</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>TSSOP-10_3x3mm_P0.5mm</t>
+  </si>
+  <si>
+    <t>https://www.onsemi.com/pub/Collateral/FSUSB42-D.PDF</t>
   </si>
   <si>
     <t>41</t>
   </si>
   <si>
-    <t>AP64351</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>AP64501SP-13</t>
-  </si>
-  <si>
-    <t>SOIC-8-1EP_3.9x4.9mm_P1.27mm_EP2.95x4.9mm_Mask2.71x3.4mm_ThermalVias</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AP64501.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AP64501SP-13/10419715</t>
+    <t>NCP1117-3.3_SOT223</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>SOT-223-3_TabPin2</t>
+  </si>
+  <si>
+    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
   </si>
   <si>
     <t>42</t>
   </si>
   <si>
-    <t>Low-Power, Two-Port, High-Speed, USB2.0 (480Mbps) or UART Switch, MSOP-10</t>
-  </si>
-  <si>
-    <t>FSUSB42MUX</t>
-  </si>
-  <si>
-    <t>U8</t>
-  </si>
-  <si>
-    <t>MSOP-10_3x3mm_P0.5mm</t>
-  </si>
-  <si>
-    <t>https://www.onsemi.com/pub/Collateral/FSUSB42-D.PDF</t>
+    <t>RP2040</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>RP2040-QFN-56</t>
+  </si>
+  <si>
+    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
   </si>
   <si>
     <t>43</t>
   </si>
   <si>
-    <t>NCP1117-3.3_SOT223</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>SOT-223-3_TabPin2</t>
-  </si>
-  <si>
-    <t>https://www.diodes.com/assets/Datasheets/AZ1117I.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
+    <t>TLP2761</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>SO-6L_10x3.84mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
   </si>
   <si>
     <t>44</t>
   </si>
   <si>
-    <t>RP2040</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>RP2040-QFN-56</t>
-  </si>
-  <si>
-    <t>https://datasheets.raspberrypi.com/rp2040/rp2040-datasheet.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/raspberry-pi/SC0914-13/14306010</t>
+    <t>USB 2.0 Hi-Speed Hub Controller</t>
+  </si>
+  <si>
+    <t>USB2514B_Bi</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>QFN-36-1EP_6x6mm_P0.5mm_EP3.7x3.7mm</t>
+  </si>
+  <si>
+    <t>http://ww1.microchip.com/downloads/en/DeviceDoc/00001692C.pdf</t>
   </si>
   <si>
     <t>45</t>
   </si>
   <si>
-    <t>TLP2761</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>SO-6L_10x3.84mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://toshiba.semicon-storage.com/info/docget.jsp?did=28819&amp;prodName=TLP2761</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/toshiba-semiconductor-and-storage/TLP2761-TP-E/7809713</t>
+    <t>W25Q128JVS-Memory_Flash</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>W25Q128JVS</t>
+  </si>
+  <si>
+    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
   </si>
   <si>
     <t>46</t>
   </si>
   <si>
-    <t>USB 2.0 Hi-Speed Hub Controller</t>
-  </si>
-  <si>
-    <t>USB2514B_Bi</t>
-  </si>
-  <si>
-    <t>U9</t>
-  </si>
-  <si>
-    <t>QFN-36-1EP_6x6mm_P0.5mm_EP3.7x3.7mm</t>
-  </si>
-  <si>
-    <t>http://ww1.microchip.com/downloads/en/DeviceDoc/00001692C.pdf</t>
+    <t>ABM8-272-T3</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>ABM8-272-T3_ABR</t>
+  </si>
+  <si>
+    <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/6387/ABM8_272_T3-3392615-pages.pdf</t>
   </si>
   <si>
     <t>47</t>
   </si>
   <si>
-    <t>W25Q128JVS-Memory_Flash</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>W25Q128JVS</t>
-  </si>
-  <si>
-    <t>SOIC-8_5.23x5.23mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>https://www.winbond.com/resource-files/w25q128jv%20revf%2003272018%20plus.pdf</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ch/de/products/detail/winbond-electronics/W25Q128JVSIQ-TR/5803944</t>
-  </si>
-  <si>
-    <t>48</t>
-  </si>
-  <si>
-    <t>ABM8-272-T3</t>
-  </si>
-  <si>
-    <t>X1</t>
-  </si>
-  <si>
-    <t>ABM8-272-T3_ABR</t>
-  </si>
-  <si>
-    <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/6387/ABM8_272_T3-3392615-pages.pdf</t>
-  </si>
-  <si>
-    <t>49</t>
-  </si>
-  <si>
     <t>Two pin crystal, small symbol</t>
   </si>
   <si>
@@ -934,7 +901,7 @@
     <t>Y1</t>
   </si>
   <si>
-    <t>Crystal_SMD_HC49-SD</t>
+    <t>Crystal_SMD_5032-2Pin_5.0x3.2mm</t>
   </si>
   <si>
     <t>KiBot Bill of Materials</t>
@@ -976,13 +943,13 @@
     <t>Component Count:</t>
   </si>
   <si>
-    <t>130 (96 SMD/ 20 THT)</t>
+    <t>133 (112 SMD/ 20 THT)</t>
   </si>
   <si>
     <t>Fitted Components:</t>
   </si>
   <si>
-    <t>120 (93 SMD/ 13 THT)</t>
+    <t>123 (109 SMD/ 13 THT)</t>
   </si>
   <si>
     <t>Number of PCBs:</t>
@@ -1633,7 +1600,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -1661,7 +1628,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1678,55 +1645,55 @@
     </row>
     <row r="2" spans="1:15">
       <c r="C2" s="2" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="F2" s="3">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="C3" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="C4" s="2" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="C5" s="2" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -1734,16 +1701,16 @@
     </row>
     <row r="6" spans="1:15">
       <c r="C6" s="2" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="F6" s="3">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -2312,22 +2279,22 @@
     </row>
     <row r="20" spans="1:15" ht="30" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>15</v>
@@ -2336,10 +2303,10 @@
         <v>22</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="K20" s="10" t="s">
         <v>16</v>
@@ -2359,37 +2326,37 @@
     </row>
     <row r="21" spans="1:15" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>94</v>
+        <v>95</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="L21" s="6" t="s">
         <v>16</v>
@@ -2406,22 +2373,22 @@
     </row>
     <row r="22" spans="1:15" ht="30" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>15</v>
@@ -2430,10 +2397,10 @@
         <v>22</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K22" s="10" t="s">
         <v>16</v>
@@ -2453,22 +2420,22 @@
     </row>
     <row r="23" spans="1:15" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>15</v>
@@ -2477,7 +2444,7 @@
         <v>22</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J23" s="8" t="s">
         <v>108</v>
@@ -2500,37 +2467,37 @@
     </row>
     <row r="24" spans="1:15" ht="30" customHeight="1">
       <c r="A24" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="B24" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="11" t="s">
+      <c r="D24" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="E24" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="F24" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="G24" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>107</v>
       </c>
       <c r="J24" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="K24" s="10" t="s">
-        <v>16</v>
+      <c r="K24" s="12" t="s">
+        <v>115</v>
       </c>
       <c r="L24" s="10" t="s">
         <v>16</v>
@@ -2547,37 +2514,37 @@
     </row>
     <row r="25" spans="1:15" ht="30" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L25" s="6" t="s">
         <v>16</v>
@@ -2592,71 +2559,71 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="30" customHeight="1">
+    <row r="26" spans="1:15">
       <c r="A26" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="J26" s="12" t="s">
+      <c r="I26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O26" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="30" customHeight="1">
+      <c r="A27" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="K26" s="12" t="s">
+      <c r="B27" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="L26" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="M26" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="N26" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="O26" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15">
-      <c r="A27" s="5" t="s">
+      <c r="D27" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="7" t="s">
+      <c r="E27" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F27" s="7" t="s">
         <v>132</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>135</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>15</v>
@@ -2665,10 +2632,10 @@
         <v>22</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>16</v>
+        <v>78</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>133</v>
       </c>
       <c r="K27" s="6" t="s">
         <v>16</v>
@@ -2686,12 +2653,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="30" customHeight="1">
+    <row r="28" spans="1:15">
       <c r="A28" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>16</v>
+        <v>134</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>135</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>136</v>
@@ -2714,8 +2681,8 @@
       <c r="I28" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="J28" s="12" t="s">
-        <v>139</v>
+      <c r="J28" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="K28" s="10" t="s">
         <v>16</v>
@@ -2735,22 +2702,22 @@
     </row>
     <row r="29" spans="1:15">
       <c r="A29" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="D29" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>143</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>15</v>
@@ -2782,25 +2749,25 @@
     </row>
     <row r="30" spans="1:15" ht="30" customHeight="1">
       <c r="A30" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" s="11" t="s">
+      <c r="D30" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="D30" s="11" t="s">
+      <c r="E30" s="11" t="s">
         <v>146</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>145</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>147</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>22</v>
@@ -2827,24 +2794,24 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" ht="30" customHeight="1">
       <c r="A31" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="D31" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="E31" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>16</v>
+      <c r="F31" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>15</v>
@@ -2852,14 +2819,14 @@
       <c r="H31" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I31" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="J31" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>16</v>
+      <c r="I31" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>157</v>
       </c>
       <c r="L31" s="6" t="s">
         <v>16</v>
@@ -2876,34 +2843,34 @@
     </row>
     <row r="32" spans="1:15" ht="30" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="H32" s="9" t="s">
         <v>22</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="J32" s="12" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="K32" s="10" t="s">
         <v>16</v>
@@ -2923,37 +2890,37 @@
     </row>
     <row r="33" spans="1:15" ht="30" customHeight="1">
       <c r="A33" s="5" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="K33" s="8" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="L33" s="6" t="s">
         <v>16</v>
@@ -2970,34 +2937,34 @@
     </row>
     <row r="34" spans="1:15" ht="30" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G34" s="9" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H34" s="9" t="s">
         <v>22</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="J34" s="12" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="K34" s="10" t="s">
         <v>16</v>
@@ -3017,37 +2984,37 @@
     </row>
     <row r="35" spans="1:15" ht="30" customHeight="1">
       <c r="A35" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I35" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I35" s="7" t="s">
+      <c r="J35" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="J35" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="K35" s="8" t="s">
-        <v>182</v>
+      <c r="K35" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="L35" s="6" t="s">
         <v>16</v>
@@ -3064,225 +3031,225 @@
     </row>
     <row r="36" spans="1:15" ht="30" customHeight="1">
       <c r="A36" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="E36" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="B36" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="D36" s="11" t="s">
+      <c r="F36" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="J36" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="K36" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L36" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M36" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N36" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O36" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="60" customHeight="1">
+      <c r="A37" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="F36" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="G36" s="9" t="s">
+      <c r="B37" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M37" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N37" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O37" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="60" customHeight="1">
+      <c r="A38" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="K38" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="L38" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M38" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N38" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O38" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="30" customHeight="1">
+      <c r="A39" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="G39" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H36" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I36" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="J36" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="K36" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="L36" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="M36" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="N36" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="O36" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="30" customHeight="1">
-      <c r="A37" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I37" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="K37" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L37" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="M37" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="N37" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O37" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="30" customHeight="1">
-      <c r="A38" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="F38" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I38" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="J38" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="K38" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="L38" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="M38" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="N38" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="O38" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="60" customHeight="1">
-      <c r="A39" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="D39" s="7" t="s">
+      <c r="H39" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J39" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="K39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O39" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="30" customHeight="1">
+      <c r="A40" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="F39" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="J39" s="8" t="s">
+      <c r="B40" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D40" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="K39" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L39" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="M39" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="N39" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O39" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="60" customHeight="1">
-      <c r="A40" s="9" t="s">
+      <c r="E40" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="D40" s="11" t="s">
+      <c r="F40" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I40" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="E40" s="11" t="s">
+      <c r="J40" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="F40" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I40" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="J40" s="12" t="s">
+      <c r="K40" s="12" t="s">
         <v>203</v>
-      </c>
-      <c r="K40" s="12" t="s">
-        <v>204</v>
       </c>
       <c r="L40" s="10" t="s">
         <v>16</v>
@@ -3299,37 +3266,37 @@
     </row>
     <row r="41" spans="1:15" ht="30" customHeight="1">
       <c r="A41" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D41" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="D41" s="7" t="s">
+      <c r="E41" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="F41" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="J41" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="F41" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I41" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="J41" s="8" t="s">
+      <c r="K41" s="8" t="s">
         <v>208</v>
-      </c>
-      <c r="K41" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="L41" s="6" t="s">
         <v>16</v>
@@ -3352,7 +3319,7 @@
         <v>16</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>210</v>
@@ -3361,22 +3328,22 @@
         <v>211</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="H42" s="9" t="s">
         <v>22</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>212</v>
+        <v>169</v>
       </c>
       <c r="J42" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="K42" s="12" t="s">
-        <v>214</v>
+        <v>202</v>
+      </c>
+      <c r="K42" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="L42" s="10" t="s">
         <v>16</v>
@@ -3393,31 +3360,31 @@
     </row>
     <row r="43" spans="1:15" ht="30" customHeight="1">
       <c r="A43" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="D43" s="7" t="s">
+      <c r="F43" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="G43" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I43" s="7" t="s">
         <v>217</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>186</v>
       </c>
       <c r="J43" s="8" t="s">
         <v>218</v>
@@ -3446,31 +3413,31 @@
         <v>16</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>176</v>
+        <v>221</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E44" s="11" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>179</v>
+        <v>224</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H44" s="9" t="s">
         <v>22</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>180</v>
+        <v>225</v>
       </c>
       <c r="J44" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="K44" s="10" t="s">
-        <v>16</v>
+        <v>226</v>
+      </c>
+      <c r="K44" s="12" t="s">
+        <v>227</v>
       </c>
       <c r="L44" s="10" t="s">
         <v>16</v>
@@ -3487,22 +3454,22 @@
     </row>
     <row r="45" spans="1:15" ht="30" customHeight="1">
       <c r="A45" s="5" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>21</v>
@@ -3511,13 +3478,13 @@
         <v>22</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="J45" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="K45" s="8" t="s">
-        <v>230</v>
+        <v>233</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="L45" s="6" t="s">
         <v>16</v>
@@ -3532,83 +3499,83 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="30" customHeight="1">
+    <row r="46" spans="1:15">
       <c r="A46" s="9" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F46" s="11" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="H46" s="9" t="s">
         <v>22</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="J46" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="K46" s="12" t="s">
         <v>238</v>
       </c>
+      <c r="J46" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K46" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="L46" s="10" t="s">
         <v>16</v>
       </c>
       <c r="M46" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="N46" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="O46" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" ht="30" customHeight="1">
+      <c r="N46" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O46" s="12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="45" customHeight="1">
       <c r="A47" s="5" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>22</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="J47" s="8" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="K47" s="6" t="s">
         <v>16</v>
@@ -3626,24 +3593,24 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" ht="30" customHeight="1">
       <c r="A48" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>16</v>
+        <v>247</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>248</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>15</v>
@@ -3652,7 +3619,7 @@
         <v>22</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="J48" s="10" t="s">
         <v>16</v>
@@ -3666,31 +3633,31 @@
       <c r="M48" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="N48" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="O48" s="12" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" ht="45" customHeight="1">
+      <c r="N48" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O48" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="30" customHeight="1">
       <c r="A49" s="5" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E49" s="7" t="s">
         <v>254</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>15</v>
@@ -3699,10 +3666,10 @@
         <v>22</v>
       </c>
       <c r="I49" s="7" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="J49" s="8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="K49" s="6" t="s">
         <v>16</v>
@@ -3722,10 +3689,10 @@
     </row>
     <row r="50" spans="1:15" ht="30" customHeight="1">
       <c r="A50" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="B50" s="12" t="s">
         <v>259</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>260</v>
@@ -3748,8 +3715,8 @@
       <c r="I50" s="11" t="s">
         <v>263</v>
       </c>
-      <c r="J50" s="10" t="s">
-        <v>16</v>
+      <c r="J50" s="12" t="s">
+        <v>264</v>
       </c>
       <c r="K50" s="10" t="s">
         <v>16</v>
@@ -3769,22 +3736,22 @@
     </row>
     <row r="51" spans="1:15" ht="30" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D51" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="E51" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="E51" s="7" t="s">
-        <v>265</v>
-      </c>
       <c r="F51" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>15</v>
@@ -3793,10 +3760,10 @@
         <v>22</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J51" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="K51" s="6" t="s">
         <v>16</v>
@@ -3816,22 +3783,22 @@
     </row>
     <row r="52" spans="1:15" ht="30" customHeight="1">
       <c r="A52" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>16</v>
+        <v>271</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>272</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="G52" s="9" t="s">
         <v>15</v>
@@ -3840,10 +3807,10 @@
         <v>22</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>274</v>
-      </c>
-      <c r="J52" s="12" t="s">
-        <v>275</v>
+        <v>276</v>
+      </c>
+      <c r="J52" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="K52" s="10" t="s">
         <v>16</v>
@@ -3863,22 +3830,22 @@
     </row>
     <row r="53" spans="1:15" ht="30" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>15</v>
@@ -3887,10 +3854,10 @@
         <v>22</v>
       </c>
       <c r="I53" s="7" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="J53" s="8" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="K53" s="6" t="s">
         <v>16</v>
@@ -3910,22 +3877,22 @@
     </row>
     <row r="54" spans="1:15" ht="30" customHeight="1">
       <c r="A54" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>283</v>
+        <v>284</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D54" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="E54" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="E54" s="11" t="s">
-        <v>284</v>
-      </c>
       <c r="F54" s="11" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G54" s="9" t="s">
         <v>15</v>
@@ -3934,7 +3901,7 @@
         <v>22</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J54" s="10" t="s">
         <v>16</v>
@@ -3955,24 +3922,24 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="30" customHeight="1">
+    <row r="55" spans="1:15">
       <c r="A55" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>16</v>
+        <v>289</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>290</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="E55" s="7" t="s">
         <v>291</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>15</v>
@@ -3980,11 +3947,11 @@
       <c r="H55" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I55" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="J55" s="8" t="s">
-        <v>294</v>
+      <c r="I55" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="K55" s="6" t="s">
         <v>16</v>
@@ -3999,100 +3966,6 @@
         <v>16</v>
       </c>
       <c r="O55" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" ht="30" customHeight="1">
-      <c r="A56" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="B56" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>296</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>297</v>
-      </c>
-      <c r="E56" s="11" t="s">
-        <v>296</v>
-      </c>
-      <c r="F56" s="11" t="s">
-        <v>298</v>
-      </c>
-      <c r="G56" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H56" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I56" s="11" t="s">
-        <v>299</v>
-      </c>
-      <c r="J56" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K56" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="L56" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="M56" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="N56" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="O56" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15">
-      <c r="A57" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H57" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I57" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="J57" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K57" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="L57" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="M57" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="N57" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O57" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -4136,7 +4009,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4153,55 +4026,55 @@
     </row>
     <row r="2" spans="1:15">
       <c r="C2" s="2" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="F2" s="3">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="C3" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="C4" s="2" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="C5" s="2" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -4209,16 +4082,16 @@
     </row>
     <row r="6" spans="1:15">
       <c r="C6" s="2" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="F6" s="3">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -4276,28 +4149,28 @@
         <v>16</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>15</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="K9" s="6" t="s">
         <v>16</v>
@@ -4323,31 +4196,31 @@
         <v>16</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>21</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="L10" s="10" t="s">
         <v>16</v>
@@ -4370,22 +4243,22 @@
         <v>16</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>21</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="I11" s="6" t="s">
         <v>78</v>
@@ -4417,28 +4290,28 @@
         <v>16</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>21</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="K12" s="10" t="s">
         <v>16</v>
@@ -4464,22 +4337,22 @@
         <v>16</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>15</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>78</v>
@@ -4511,31 +4384,31 @@
         <v>16</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>21</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="L14" s="10" t="s">
         <v>16</v>
@@ -4573,27 +4446,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="7" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="6" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>